<commit_message>
new experiments with openai
</commit_message>
<xml_diff>
--- a/experiment_results/10428P6.xlsx
+++ b/experiment_results/10428P6.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I967"/>
+  <dimension ref="A1:I1112"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -771,7 +771,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Category: ['Dining Experiences', 'Culinary Tours']</t>
+          <t>Category: ['Culinary Tours', 'Dining Experiences']</t>
         </is>
       </c>
       <c r="B19" t="inlineStr"/>
@@ -921,7 +921,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Category: ['Historical Tours', 'City Tours']</t>
+          <t>Category: ['City Tours', 'Historical Tours']</t>
         </is>
       </c>
       <c r="B29" t="inlineStr"/>
@@ -996,7 +996,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Category: ['Modern Attractions', 'City Tours']</t>
+          <t>Category: ['City Tours', 'Modern Attractions']</t>
         </is>
       </c>
       <c r="B34" t="inlineStr"/>
@@ -1071,7 +1071,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Category: ['Historical Tours', 'City Tours']</t>
+          <t>Category: ['City Tours', 'Historical Tours']</t>
         </is>
       </c>
       <c r="B39" t="inlineStr"/>
@@ -1146,7 +1146,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Category: ['Historical Tours', 'City Tours']</t>
+          <t>Category: ['City Tours', 'Historical Tours']</t>
         </is>
       </c>
       <c r="B44" t="inlineStr"/>
@@ -1221,7 +1221,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Category: ['Water Sports', 'Scenic Tours']</t>
+          <t>Category: ['Scenic Tours', 'Water Sports']</t>
         </is>
       </c>
       <c r="B49" t="inlineStr"/>
@@ -1371,7 +1371,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Category: ['Water Sports', 'Scenic Tours']</t>
+          <t>Category: ['Scenic Tours', 'Water Sports']</t>
         </is>
       </c>
       <c r="B59" t="inlineStr"/>
@@ -1446,7 +1446,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Category: ['Eco-Tours', 'Scenic Tours']</t>
+          <t>Category: ['Scenic Tours', 'Eco-Tours']</t>
         </is>
       </c>
       <c r="B64" t="inlineStr"/>
@@ -1671,7 +1671,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Category: ['Water Sports', 'Scenic Tours']</t>
+          <t>Category: ['Scenic Tours', 'Water Sports']</t>
         </is>
       </c>
       <c r="B79" t="inlineStr"/>
@@ -1746,7 +1746,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Category: ['Wildlife Tours', 'Scenic Tours']</t>
+          <t>Category: ['Scenic Tours', 'Wildlife Tours']</t>
         </is>
       </c>
       <c r="B84" t="inlineStr"/>
@@ -1971,7 +1971,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Category: ['Historical Tours', 'City Tours']</t>
+          <t>Category: ['City Tours', 'Historical Tours']</t>
         </is>
       </c>
       <c r="B99" t="inlineStr"/>
@@ -2046,7 +2046,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Category: ['Historical Tours', 'Cultural Tours', 'Culinary Tours']</t>
+          <t>Category: ['Historical Tours', 'Culinary Tours', 'Cultural Tours']</t>
         </is>
       </c>
       <c r="B104" t="inlineStr"/>
@@ -2196,7 +2196,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Category: ['Culinary Tours', 'City Tours']</t>
+          <t>Category: ['City Tours', 'Culinary Tours']</t>
         </is>
       </c>
       <c r="B114" t="inlineStr"/>
@@ -2346,7 +2346,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>Category: ['Scenic Tours', 'City Tours']</t>
+          <t>Category: ['City Tours', 'Scenic Tours']</t>
         </is>
       </c>
       <c r="B124" t="inlineStr"/>
@@ -2421,7 +2421,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>Category: ['Culinary Tours', 'City Tours']</t>
+          <t>Category: ['City Tours', 'Culinary Tours']</t>
         </is>
       </c>
       <c r="B129" t="inlineStr"/>
@@ -2496,7 +2496,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>Category: ['Water Sports', 'Scenic Tours']</t>
+          <t>Category: ['Scenic Tours', 'Water Sports']</t>
         </is>
       </c>
       <c r="B134" t="inlineStr"/>
@@ -2721,7 +2721,7 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>Category: ['Historical Tours', 'Culinary Tours', 'City Tours']</t>
+          <t>Category: ['City Tours', 'Historical Tours', 'Culinary Tours']</t>
         </is>
       </c>
       <c r="B149" t="inlineStr"/>
@@ -2796,7 +2796,7 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>Category: ['Dining Experiences', 'City Tours']</t>
+          <t>Category: ['City Tours', 'Dining Experiences']</t>
         </is>
       </c>
       <c r="B154" t="inlineStr"/>
@@ -3171,7 +3171,7 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>Category: ['Cultural Tours', 'City Tours']</t>
+          <t>Category: ['City Tours', 'Cultural Tours']</t>
         </is>
       </c>
       <c r="B179" t="inlineStr"/>
@@ -3321,7 +3321,7 @@
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>Category: ['Scenic Tours', 'City Tours']</t>
+          <t>Category: ['City Tours', 'Scenic Tours']</t>
         </is>
       </c>
       <c r="B189" t="inlineStr"/>
@@ -3471,7 +3471,7 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>Category: ['Culinary Tours', 'City Tours']</t>
+          <t>Category: ['City Tours', 'Culinary Tours']</t>
         </is>
       </c>
       <c r="B199" t="inlineStr"/>
@@ -3621,7 +3621,7 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>Category: ['Workshops and Classes', 'Wine and Beverage Tastings']</t>
+          <t>Category: ['Wine and Beverage Tastings', 'Workshops and Classes']</t>
         </is>
       </c>
       <c r="B209" t="inlineStr"/>
@@ -3696,7 +3696,7 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>Category: ['Entertainment', 'City Tours']</t>
+          <t>Category: ['City Tours', 'Entertainment']</t>
         </is>
       </c>
       <c r="B214" t="inlineStr"/>
@@ -3921,7 +3921,7 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>Category: ['Scenic Tours', 'City Tours']</t>
+          <t>Category: ['City Tours', 'Scenic Tours']</t>
         </is>
       </c>
       <c r="B229" t="inlineStr"/>
@@ -4521,7 +4521,7 @@
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>Category: ['Culinary Tours', 'City Tours']</t>
+          <t>Category: ['City Tours', 'Culinary Tours']</t>
         </is>
       </c>
       <c r="B269" t="inlineStr"/>
@@ -4596,7 +4596,7 @@
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>Category: ['Adventure Sports', 'Dining Experiences']</t>
+          <t>Category: ['Dining Experiences', 'Adventure Sports']</t>
         </is>
       </c>
       <c r="B274" t="inlineStr"/>
@@ -4821,7 +4821,7 @@
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>Category: ['Entertainment', 'City Tours']</t>
+          <t>Category: ['City Tours', 'Entertainment']</t>
         </is>
       </c>
       <c r="B289" t="inlineStr"/>
@@ -4971,7 +4971,7 @@
     <row r="299">
       <c r="A299" t="inlineStr">
         <is>
-          <t>Category: ['Modern Attractions', 'City Tours']</t>
+          <t>Category: ['City Tours', 'Modern Attractions']</t>
         </is>
       </c>
       <c r="B299" t="inlineStr"/>
@@ -5271,7 +5271,7 @@
     <row r="319">
       <c r="A319" t="inlineStr">
         <is>
-          <t>Category: ['Cultural Cruises', 'Spa and Wellness']</t>
+          <t>Category: ['Spa and Wellness', 'Cultural Cruises']</t>
         </is>
       </c>
       <c r="B319" t="inlineStr"/>
@@ -5346,7 +5346,7 @@
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>Category: ['Cultural Tours', 'City Tours']</t>
+          <t>Category: ['City Tours', 'Cultural Tours']</t>
         </is>
       </c>
       <c r="B324" t="inlineStr"/>
@@ -5421,7 +5421,7 @@
     <row r="329">
       <c r="A329" t="inlineStr">
         <is>
-          <t>Category: ['Aerial Tours', 'Scenic Tours']</t>
+          <t>Category: ['Scenic Tours', 'Aerial Tours']</t>
         </is>
       </c>
       <c r="B329" t="inlineStr"/>
@@ -5571,7 +5571,7 @@
     <row r="339">
       <c r="A339" t="inlineStr">
         <is>
-          <t>Category: ['Historical Tours', 'City Tours']</t>
+          <t>Category: ['City Tours', 'Historical Tours']</t>
         </is>
       </c>
       <c r="B339" t="inlineStr"/>
@@ -5721,7 +5721,7 @@
     <row r="349">
       <c r="A349" t="inlineStr">
         <is>
-          <t>Category: ['Water Sports', 'Scenic Tours']</t>
+          <t>Category: ['Scenic Tours', 'Water Sports']</t>
         </is>
       </c>
       <c r="B349" t="inlineStr"/>
@@ -5796,7 +5796,7 @@
     <row r="354">
       <c r="A354" t="inlineStr">
         <is>
-          <t>Category: ['Dining Experiences', 'City Tours']</t>
+          <t>Category: ['City Tours', 'Dining Experiences']</t>
         </is>
       </c>
       <c r="B354" t="inlineStr"/>
@@ -5871,7 +5871,7 @@
     <row r="359">
       <c r="A359" t="inlineStr">
         <is>
-          <t>Category: ['Water Sports', 'Scenic Tours']</t>
+          <t>Category: ['Scenic Tours', 'Water Sports']</t>
         </is>
       </c>
       <c r="B359" t="inlineStr"/>
@@ -6096,7 +6096,7 @@
     <row r="374">
       <c r="A374" t="inlineStr">
         <is>
-          <t>Category: ['Culinary Tours', 'Scenic Tours']</t>
+          <t>Category: ['Scenic Tours', 'Culinary Tours']</t>
         </is>
       </c>
       <c r="B374" t="inlineStr"/>
@@ -6171,7 +6171,7 @@
     <row r="379">
       <c r="A379" t="inlineStr">
         <is>
-          <t>Category: ['Entertainment', 'City Tours']</t>
+          <t>Category: ['City Tours', 'Entertainment']</t>
         </is>
       </c>
       <c r="B379" t="inlineStr"/>
@@ -6246,7 +6246,7 @@
     <row r="384">
       <c r="A384" t="inlineStr">
         <is>
-          <t>Category: ['Water Sports', 'Scenic Tours']</t>
+          <t>Category: ['Scenic Tours', 'Water Sports']</t>
         </is>
       </c>
       <c r="B384" t="inlineStr"/>
@@ -6396,7 +6396,7 @@
     <row r="394">
       <c r="A394" t="inlineStr">
         <is>
-          <t>Category: ['Hiking', 'City Tours']</t>
+          <t>Category: ['City Tours', 'Hiking']</t>
         </is>
       </c>
       <c r="B394" t="inlineStr"/>
@@ -6546,7 +6546,7 @@
     <row r="404">
       <c r="A404" t="inlineStr">
         <is>
-          <t>Category: ['Water Sports', 'Scenic Tours']</t>
+          <t>Category: ['Scenic Tours', 'Water Sports']</t>
         </is>
       </c>
       <c r="B404" t="inlineStr"/>
@@ -6621,7 +6621,7 @@
     <row r="409">
       <c r="A409" t="inlineStr">
         <is>
-          <t>Category: ['Scenic Tours', 'City Tours']</t>
+          <t>Category: ['City Tours', 'Scenic Tours']</t>
         </is>
       </c>
       <c r="B409" t="inlineStr"/>
@@ -6696,7 +6696,7 @@
     <row r="414">
       <c r="A414" t="inlineStr">
         <is>
-          <t>Category: ['Water Sports', 'Scenic Tours']</t>
+          <t>Category: ['Scenic Tours', 'Water Sports']</t>
         </is>
       </c>
       <c r="B414" t="inlineStr"/>
@@ -6771,7 +6771,7 @@
     <row r="419">
       <c r="A419" t="inlineStr">
         <is>
-          <t>Category: ['Scenic Tours', 'City Tours']</t>
+          <t>Category: ['City Tours', 'Scenic Tours']</t>
         </is>
       </c>
       <c r="B419" t="inlineStr"/>
@@ -6996,7 +6996,7 @@
     <row r="434">
       <c r="A434" t="inlineStr">
         <is>
-          <t>Category: ['Cultural Tours', 'Culinary Tours']</t>
+          <t>Category: ['Culinary Tours', 'Cultural Tours']</t>
         </is>
       </c>
       <c r="B434" t="inlineStr"/>
@@ -7221,7 +7221,7 @@
     <row r="449">
       <c r="A449" t="inlineStr">
         <is>
-          <t>Category: ['Culinary Tours', 'City Tours']</t>
+          <t>Category: ['City Tours', 'Culinary Tours']</t>
         </is>
       </c>
       <c r="B449" t="inlineStr"/>
@@ -7296,7 +7296,7 @@
     <row r="454">
       <c r="A454" t="inlineStr">
         <is>
-          <t>Category: ['Cultural Cruises', 'Scenic Tours']</t>
+          <t>Category: ['Scenic Tours', 'Cultural Cruises']</t>
         </is>
       </c>
       <c r="B454" t="inlineStr"/>
@@ -7446,7 +7446,7 @@
     <row r="464">
       <c r="A464" t="inlineStr">
         <is>
-          <t>Category: ['Scenic Tours', 'City Tours']</t>
+          <t>Category: ['City Tours', 'Scenic Tours']</t>
         </is>
       </c>
       <c r="B464" t="inlineStr"/>
@@ -7821,7 +7821,7 @@
     <row r="489">
       <c r="A489" t="inlineStr">
         <is>
-          <t>Category: ['Adventure Sports', 'Entertainment']</t>
+          <t>Category: ['Entertainment', 'Adventure Sports']</t>
         </is>
       </c>
       <c r="B489" t="inlineStr"/>
@@ -7896,7 +7896,7 @@
     <row r="494">
       <c r="A494" t="inlineStr">
         <is>
-          <t>Category: ['Water Sports', 'Scenic Tours']</t>
+          <t>Category: ['Scenic Tours', 'Water Sports']</t>
         </is>
       </c>
       <c r="B494" t="inlineStr"/>
@@ -7971,7 +7971,7 @@
     <row r="499">
       <c r="A499" t="inlineStr">
         <is>
-          <t>Category: ['Cultural Tours', 'City Tours', 'Scenic Tours']</t>
+          <t>Category: ['City Tours', 'Scenic Tours', 'Cultural Tours']</t>
         </is>
       </c>
       <c r="B499" t="inlineStr"/>
@@ -8121,7 +8121,7 @@
     <row r="509">
       <c r="A509" t="inlineStr">
         <is>
-          <t>Category: ['Cultural Tours', 'City Tours']</t>
+          <t>Category: ['City Tours', 'Cultural Tours']</t>
         </is>
       </c>
       <c r="B509" t="inlineStr"/>
@@ -8271,7 +8271,7 @@
     <row r="519">
       <c r="A519" t="inlineStr">
         <is>
-          <t>Category: ['Cultural Cruises', 'Scenic Tours']</t>
+          <t>Category: ['Scenic Tours', 'Cultural Cruises']</t>
         </is>
       </c>
       <c r="B519" t="inlineStr"/>
@@ -8421,7 +8421,7 @@
     <row r="529">
       <c r="A529" t="inlineStr">
         <is>
-          <t>Category: ['Hiking', 'Culinary Tours', 'City Tours']</t>
+          <t>Category: ['City Tours', 'Hiking', 'Culinary Tours']</t>
         </is>
       </c>
       <c r="B529" t="inlineStr"/>
@@ -8571,7 +8571,7 @@
     <row r="539">
       <c r="A539" t="inlineStr">
         <is>
-          <t>Category: ['Shopping and Fashion', 'City Tours']</t>
+          <t>Category: ['City Tours', 'Shopping and Fashion']</t>
         </is>
       </c>
       <c r="B539" t="inlineStr"/>
@@ -8796,7 +8796,7 @@
     <row r="554">
       <c r="A554" t="inlineStr">
         <is>
-          <t>Category: ['Scenic Tours', 'Hiking']</t>
+          <t>Category: ['Hiking', 'Scenic Tours']</t>
         </is>
       </c>
       <c r="B554" t="inlineStr"/>
@@ -9171,7 +9171,7 @@
     <row r="579">
       <c r="A579" t="inlineStr">
         <is>
-          <t>Category: ['Historical Tours', 'City Tours']</t>
+          <t>Category: ['City Tours', 'Historical Tours']</t>
         </is>
       </c>
       <c r="B579" t="inlineStr"/>
@@ -9246,7 +9246,7 @@
     <row r="584">
       <c r="A584" t="inlineStr">
         <is>
-          <t>Category: ['Water Sports', 'Scenic Tours']</t>
+          <t>Category: ['Scenic Tours', 'Water Sports']</t>
         </is>
       </c>
       <c r="B584" t="inlineStr"/>
@@ -9696,7 +9696,7 @@
     <row r="614">
       <c r="A614" t="inlineStr">
         <is>
-          <t>Category: ['Modern Attractions', 'City Tours']</t>
+          <t>Category: ['City Tours', 'Modern Attractions']</t>
         </is>
       </c>
       <c r="B614" t="inlineStr"/>
@@ -9846,7 +9846,7 @@
     <row r="624">
       <c r="A624" t="inlineStr">
         <is>
-          <t>Category: ['Water Sports', 'Scenic Tours']</t>
+          <t>Category: ['Scenic Tours', 'Water Sports']</t>
         </is>
       </c>
       <c r="B624" t="inlineStr"/>
@@ -9921,7 +9921,7 @@
     <row r="629">
       <c r="A629" t="inlineStr">
         <is>
-          <t>Category: ['Cultural Tours', 'City Tours']</t>
+          <t>Category: ['City Tours', 'Cultural Tours']</t>
         </is>
       </c>
       <c r="B629" t="inlineStr"/>
@@ -10221,7 +10221,7 @@
     <row r="649">
       <c r="A649" t="inlineStr">
         <is>
-          <t>Category: ['Hiking', 'Cultural Tours', 'City Tours']</t>
+          <t>Category: ['City Tours', 'Hiking', 'Cultural Tours']</t>
         </is>
       </c>
       <c r="B649" t="inlineStr"/>
@@ -10371,7 +10371,7 @@
     <row r="659">
       <c r="A659" t="inlineStr">
         <is>
-          <t>Category: ['Historical Tours', 'Scenic Tours']</t>
+          <t>Category: ['Scenic Tours', 'Historical Tours']</t>
         </is>
       </c>
       <c r="B659" t="inlineStr"/>
@@ -10596,7 +10596,7 @@
     <row r="674">
       <c r="A674" t="inlineStr">
         <is>
-          <t>Category: ['Historical Tours', 'City Tours']</t>
+          <t>Category: ['City Tours', 'Historical Tours']</t>
         </is>
       </c>
       <c r="B674" t="inlineStr"/>
@@ -10896,7 +10896,7 @@
     <row r="694">
       <c r="A694" t="inlineStr">
         <is>
-          <t>Category: ['Water Sports', 'Scenic Tours']</t>
+          <t>Category: ['Scenic Tours', 'Water Sports']</t>
         </is>
       </c>
       <c r="B694" t="inlineStr"/>
@@ -10971,7 +10971,7 @@
     <row r="699">
       <c r="A699" t="inlineStr">
         <is>
-          <t>Category: ['Dining Experiences', 'Culinary Tours']</t>
+          <t>Category: ['Culinary Tours', 'Dining Experiences']</t>
         </is>
       </c>
       <c r="B699" t="inlineStr"/>
@@ -11121,7 +11121,7 @@
     <row r="709">
       <c r="A709" t="inlineStr">
         <is>
-          <t>Category: ['Entertainment', 'City Tours']</t>
+          <t>Category: ['City Tours', 'Entertainment']</t>
         </is>
       </c>
       <c r="B709" t="inlineStr"/>
@@ -11271,7 +11271,7 @@
     <row r="719">
       <c r="A719" t="inlineStr">
         <is>
-          <t>Category: ['Water Sports', 'Scenic Tours']</t>
+          <t>Category: ['Scenic Tours', 'Water Sports']</t>
         </is>
       </c>
       <c r="B719" t="inlineStr"/>
@@ -11421,7 +11421,7 @@
     <row r="729">
       <c r="A729" t="inlineStr">
         <is>
-          <t>Category: ['Scenic Tours', 'City Tours']</t>
+          <t>Category: ['City Tours', 'Scenic Tours']</t>
         </is>
       </c>
       <c r="B729" t="inlineStr"/>
@@ -11496,7 +11496,7 @@
     <row r="734">
       <c r="A734" t="inlineStr">
         <is>
-          <t>Category: ['Dining Experiences', 'Scenic Tours']</t>
+          <t>Category: ['Scenic Tours', 'Dining Experiences']</t>
         </is>
       </c>
       <c r="B734" t="inlineStr"/>
@@ -11571,7 +11571,7 @@
     <row r="739">
       <c r="A739" t="inlineStr">
         <is>
-          <t>Category: ['Dining Experiences', 'Water Sports', 'Scenic Tours']</t>
+          <t>Category: ['Scenic Tours', 'Dining Experiences', 'Water Sports']</t>
         </is>
       </c>
       <c r="B739" t="inlineStr"/>
@@ -11721,7 +11721,7 @@
     <row r="749">
       <c r="A749" t="inlineStr">
         <is>
-          <t>Category: ['Dining Experiences', 'Culinary Tours']</t>
+          <t>Category: ['Culinary Tours', 'Dining Experiences']</t>
         </is>
       </c>
       <c r="B749" t="inlineStr"/>
@@ -11796,7 +11796,7 @@
     <row r="754">
       <c r="A754" t="inlineStr">
         <is>
-          <t>Category: ['Adventure Sports', 'Water Sports']</t>
+          <t>Category: ['Water Sports', 'Adventure Sports']</t>
         </is>
       </c>
       <c r="B754" t="inlineStr"/>
@@ -11871,7 +11871,7 @@
     <row r="759">
       <c r="A759" t="inlineStr">
         <is>
-          <t>Category: ['Scenic Tours', 'Hiking']</t>
+          <t>Category: ['Hiking', 'Scenic Tours']</t>
         </is>
       </c>
       <c r="B759" t="inlineStr"/>
@@ -11946,7 +11946,7 @@
     <row r="764">
       <c r="A764" t="inlineStr">
         <is>
-          <t>Category: ['Adventure Sports', 'Water Sports']</t>
+          <t>Category: ['Water Sports', 'Adventure Sports']</t>
         </is>
       </c>
       <c r="B764" t="inlineStr"/>
@@ -12021,7 +12021,7 @@
     <row r="769">
       <c r="A769" t="inlineStr">
         <is>
-          <t>Category: ['Cultural Tours', 'Scenic Tours']</t>
+          <t>Category: ['Scenic Tours', 'Cultural Tours']</t>
         </is>
       </c>
       <c r="B769" t="inlineStr"/>
@@ -12096,7 +12096,7 @@
     <row r="774">
       <c r="A774" t="inlineStr">
         <is>
-          <t>Category: ['Adventure Sports', 'Dining Experiences']</t>
+          <t>Category: ['Dining Experiences', 'Adventure Sports']</t>
         </is>
       </c>
       <c r="B774" t="inlineStr"/>
@@ -12171,7 +12171,7 @@
     <row r="779">
       <c r="A779" t="inlineStr">
         <is>
-          <t>Category: ['Water Sports', 'Scenic Tours']</t>
+          <t>Category: ['Scenic Tours', 'Water Sports']</t>
         </is>
       </c>
       <c r="B779" t="inlineStr"/>
@@ -12321,7 +12321,7 @@
     <row r="789">
       <c r="A789" t="inlineStr">
         <is>
-          <t>Category: ['Culinary Tours', 'City Tours']</t>
+          <t>Category: ['City Tours', 'Culinary Tours']</t>
         </is>
       </c>
       <c r="B789" t="inlineStr"/>
@@ -12396,7 +12396,7 @@
     <row r="794">
       <c r="A794" t="inlineStr">
         <is>
-          <t>Category: ['Historical Tours', 'Culinary Tours', 'City Tours']</t>
+          <t>Category: ['City Tours', 'Historical Tours', 'Culinary Tours']</t>
         </is>
       </c>
       <c r="B794" t="inlineStr"/>
@@ -12621,7 +12621,7 @@
     <row r="809">
       <c r="A809" t="inlineStr">
         <is>
-          <t>Category: ['Entertainment', 'Water Sports', 'Scenic Tours']</t>
+          <t>Category: ['Scenic Tours', 'Entertainment', 'Water Sports']</t>
         </is>
       </c>
       <c r="B809" t="inlineStr"/>
@@ -12696,7 +12696,7 @@
     <row r="814">
       <c r="A814" t="inlineStr">
         <is>
-          <t>Category: ['Dining Experiences', 'Culinary Tours']</t>
+          <t>Category: ['Culinary Tours', 'Dining Experiences']</t>
         </is>
       </c>
       <c r="B814" t="inlineStr"/>
@@ -12771,7 +12771,7 @@
     <row r="819">
       <c r="A819" t="inlineStr">
         <is>
-          <t>Category: ['Historical Tours', 'City Tours']</t>
+          <t>Category: ['City Tours', 'Historical Tours']</t>
         </is>
       </c>
       <c r="B819" t="inlineStr"/>
@@ -12846,7 +12846,7 @@
     <row r="824">
       <c r="A824" t="inlineStr">
         <is>
-          <t>Category: ['Water Sports', 'Scenic Tours']</t>
+          <t>Category: ['Scenic Tours', 'Water Sports']</t>
         </is>
       </c>
       <c r="B824" t="inlineStr"/>
@@ -12996,7 +12996,7 @@
     <row r="834">
       <c r="A834" t="inlineStr">
         <is>
-          <t>Category: ['Entertainment', 'Historical Tours', 'City Tours']</t>
+          <t>Category: ['City Tours', 'Entertainment', 'Historical Tours']</t>
         </is>
       </c>
       <c r="B834" t="inlineStr"/>
@@ -13521,7 +13521,7 @@
     <row r="869">
       <c r="A869" t="inlineStr">
         <is>
-          <t>Category: ['Performing Arts', 'Entertainment', 'City Tours']</t>
+          <t>Category: ['City Tours', 'Entertainment', 'Performing Arts']</t>
         </is>
       </c>
       <c r="B869" t="inlineStr"/>
@@ -13596,7 +13596,7 @@
     <row r="874">
       <c r="A874" t="inlineStr">
         <is>
-          <t>Category: ['Culinary Tours', 'City Tours']</t>
+          <t>Category: ['City Tours', 'Culinary Tours']</t>
         </is>
       </c>
       <c r="B874" t="inlineStr"/>
@@ -13671,7 +13671,7 @@
     <row r="879">
       <c r="A879" t="inlineStr">
         <is>
-          <t>Category: ['Historical Tours', 'Scenic Tours']</t>
+          <t>Category: ['Scenic Tours', 'Historical Tours']</t>
         </is>
       </c>
       <c r="B879" t="inlineStr"/>
@@ -13746,7 +13746,7 @@
     <row r="884">
       <c r="A884" t="inlineStr">
         <is>
-          <t>Category: ['Water Sports', 'Scenic Tours']</t>
+          <t>Category: ['Scenic Tours', 'Water Sports']</t>
         </is>
       </c>
       <c r="B884" t="inlineStr"/>
@@ -13971,7 +13971,7 @@
     <row r="899">
       <c r="A899" t="inlineStr">
         <is>
-          <t>Category: ['Entertainment', 'City Tours']</t>
+          <t>Category: ['City Tours', 'Entertainment']</t>
         </is>
       </c>
       <c r="B899" t="inlineStr"/>
@@ -14121,7 +14121,7 @@
     <row r="909">
       <c r="A909" t="inlineStr">
         <is>
-          <t>Category: ['Wine and Beverage Tastings', 'Culinary Tours', 'Scenic Tours']</t>
+          <t>Category: ['Wine and Beverage Tastings', 'Scenic Tours', 'Culinary Tours']</t>
         </is>
       </c>
       <c r="B909" t="inlineStr"/>
@@ -14196,7 +14196,7 @@
     <row r="914">
       <c r="A914" t="inlineStr">
         <is>
-          <t>Category: ['Cultural Festivals', 'Cultural Tours', 'City Tours']</t>
+          <t>Category: ['City Tours', 'Cultural Festivals', 'Cultural Tours']</t>
         </is>
       </c>
       <c r="B914" t="inlineStr"/>
@@ -14346,7 +14346,7 @@
     <row r="924">
       <c r="A924" t="inlineStr">
         <is>
-          <t>Category: ['Entertainment', 'City Tours']</t>
+          <t>Category: ['City Tours', 'Entertainment']</t>
         </is>
       </c>
       <c r="B924" t="inlineStr"/>
@@ -14646,7 +14646,7 @@
     <row r="944">
       <c r="A944" t="inlineStr">
         <is>
-          <t>Category: ['Cultural Tours', 'Scenic Tours', 'City Tours']</t>
+          <t>Category: ['City Tours', 'Scenic Tours', 'Cultural Tours']</t>
         </is>
       </c>
       <c r="B944" t="inlineStr"/>
@@ -14721,7 +14721,7 @@
     <row r="949">
       <c r="A949" t="inlineStr">
         <is>
-          <t>Category: ['Adventure Sports', 'Entertainment']</t>
+          <t>Category: ['Entertainment', 'Adventure Sports']</t>
         </is>
       </c>
       <c r="B949" t="inlineStr"/>
@@ -14946,7 +14946,7 @@
     <row r="964">
       <c r="A964" t="inlineStr">
         <is>
-          <t>Category: ['Wine and Beverage Tastings', 'Culinary Tours', 'City Tours']</t>
+          <t>Category: ['City Tours', 'Culinary Tours', 'Wine and Beverage Tastings']</t>
         </is>
       </c>
       <c r="B964" t="inlineStr"/>
@@ -14992,7 +14992,7 @@
     <row r="967">
       <c r="A967" t="inlineStr">
         <is>
-          <t>*****</t>
+          <t>PRODUCTCODE: 25218P1</t>
         </is>
       </c>
       <c r="B967" t="inlineStr"/>
@@ -15004,6 +15004,2181 @@
       <c r="H967" t="inlineStr"/>
       <c r="I967" t="inlineStr"/>
     </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>Summarized description: This 4-hour brewery tour in Austin allows you to have the freedom to enjoy three local breweries. This is a great activity for bachelor and bachelorette parties, birthday parties.</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr"/>
+      <c r="C968" t="inlineStr"/>
+      <c r="D968" t="inlineStr"/>
+      <c r="E968" t="inlineStr"/>
+      <c r="F968" t="inlineStr"/>
+      <c r="G968" t="inlineStr"/>
+      <c r="H968" t="inlineStr"/>
+      <c r="I968" t="inlineStr"/>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>Title: Brewery Tour: Experience Austin in a Half Day</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr"/>
+      <c r="C969" t="inlineStr"/>
+      <c r="D969" t="inlineStr"/>
+      <c r="E969" t="inlineStr"/>
+      <c r="F969" t="inlineStr"/>
+      <c r="G969" t="inlineStr"/>
+      <c r="H969" t="inlineStr"/>
+      <c r="I969" t="inlineStr"/>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>TotalReviews: 113</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr"/>
+      <c r="C970" t="inlineStr"/>
+      <c r="D970" t="inlineStr"/>
+      <c r="E970" t="inlineStr"/>
+      <c r="F970" t="inlineStr"/>
+      <c r="G970" t="inlineStr"/>
+      <c r="H970" t="inlineStr"/>
+      <c r="I970" t="inlineStr"/>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>Category: ['Wine and Beverage Tastings', 'Culinary Tours']</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr"/>
+      <c r="C971" t="inlineStr"/>
+      <c r="D971" t="inlineStr"/>
+      <c r="E971" t="inlineStr"/>
+      <c r="F971" t="inlineStr"/>
+      <c r="G971" t="inlineStr"/>
+      <c r="H971" t="inlineStr"/>
+      <c r="I971" t="inlineStr"/>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>PRODUCTCODE: 17570P6</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr"/>
+      <c r="C972" t="inlineStr"/>
+      <c r="D972" t="inlineStr"/>
+      <c r="E972" t="inlineStr"/>
+      <c r="F972" t="inlineStr"/>
+      <c r="G972" t="inlineStr"/>
+      <c r="H972" t="inlineStr"/>
+      <c r="I972" t="inlineStr"/>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>Summarized description: Learn about Texas cowboys and the great cattle drives of the 1800s. Step back in time at the Lyndon B. Johnson State Park &amp; Historic Site. Pass by award-winning wineries &amp; orchards, before visiting Fredericksburg, a historic &amp; picturesque German town.</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr"/>
+      <c r="C973" t="inlineStr"/>
+      <c r="D973" t="inlineStr"/>
+      <c r="E973" t="inlineStr"/>
+      <c r="F973" t="inlineStr"/>
+      <c r="G973" t="inlineStr"/>
+      <c r="H973" t="inlineStr"/>
+      <c r="I973" t="inlineStr"/>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>Title: Texas Hill Country and LBJ Tour From Austin</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr"/>
+      <c r="C974" t="inlineStr"/>
+      <c r="D974" t="inlineStr"/>
+      <c r="E974" t="inlineStr"/>
+      <c r="F974" t="inlineStr"/>
+      <c r="G974" t="inlineStr"/>
+      <c r="H974" t="inlineStr"/>
+      <c r="I974" t="inlineStr"/>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>TotalReviews: 41</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr"/>
+      <c r="C975" t="inlineStr"/>
+      <c r="D975" t="inlineStr"/>
+      <c r="E975" t="inlineStr"/>
+      <c r="F975" t="inlineStr"/>
+      <c r="G975" t="inlineStr"/>
+      <c r="H975" t="inlineStr"/>
+      <c r="I975" t="inlineStr"/>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>Category: ['Historical Tours', 'Culinary Tours', 'Cultural Tours']</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr"/>
+      <c r="C976" t="inlineStr"/>
+      <c r="D976" t="inlineStr"/>
+      <c r="E976" t="inlineStr"/>
+      <c r="F976" t="inlineStr"/>
+      <c r="G976" t="inlineStr"/>
+      <c r="H976" t="inlineStr"/>
+      <c r="I976" t="inlineStr"/>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>PRODUCTCODE: 87887P1</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr"/>
+      <c r="C977" t="inlineStr"/>
+      <c r="D977" t="inlineStr"/>
+      <c r="E977" t="inlineStr"/>
+      <c r="F977" t="inlineStr"/>
+      <c r="G977" t="inlineStr"/>
+      <c r="H977" t="inlineStr"/>
+      <c r="I977" t="inlineStr"/>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>Summarized description: Lux Drift wine tour is approximately 4-6 hrs from pick up to drop off. Wine Tasting fees/bottle are NOT included in the tour price. Due to COVID19 we may change the schedule or itinerary based on state and local CDC guidance.</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr"/>
+      <c r="C978" t="inlineStr"/>
+      <c r="D978" t="inlineStr"/>
+      <c r="E978" t="inlineStr"/>
+      <c r="F978" t="inlineStr"/>
+      <c r="G978" t="inlineStr"/>
+      <c r="H978" t="inlineStr"/>
+      <c r="I978" t="inlineStr"/>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>Title: Texas Hill Country Group Wine Tour by Limousine</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr"/>
+      <c r="C979" t="inlineStr"/>
+      <c r="D979" t="inlineStr"/>
+      <c r="E979" t="inlineStr"/>
+      <c r="F979" t="inlineStr"/>
+      <c r="G979" t="inlineStr"/>
+      <c r="H979" t="inlineStr"/>
+      <c r="I979" t="inlineStr"/>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>TotalReviews: 29</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr"/>
+      <c r="C980" t="inlineStr"/>
+      <c r="D980" t="inlineStr"/>
+      <c r="E980" t="inlineStr"/>
+      <c r="F980" t="inlineStr"/>
+      <c r="G980" t="inlineStr"/>
+      <c r="H980" t="inlineStr"/>
+      <c r="I980" t="inlineStr"/>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>Category: ['Wine and Beverage Tastings']</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr"/>
+      <c r="C981" t="inlineStr"/>
+      <c r="D981" t="inlineStr"/>
+      <c r="E981" t="inlineStr"/>
+      <c r="F981" t="inlineStr"/>
+      <c r="G981" t="inlineStr"/>
+      <c r="H981" t="inlineStr"/>
+      <c r="I981" t="inlineStr"/>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>PRODUCTCODE: 199613P8</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr"/>
+      <c r="C982" t="inlineStr"/>
+      <c r="D982" t="inlineStr"/>
+      <c r="E982" t="inlineStr"/>
+      <c r="F982" t="inlineStr"/>
+      <c r="G982" t="inlineStr"/>
+      <c r="H982" t="inlineStr"/>
+      <c r="I982" t="inlineStr"/>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>Summarized description: Texas Tipsy Tours’ experience includes wine tastings or bottles to share (cost included!) at two top Texas Hill Country wineries. We will pick up and drop off at your chosen location inside Austin city limits.</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr"/>
+      <c r="C983" t="inlineStr"/>
+      <c r="D983" t="inlineStr"/>
+      <c r="E983" t="inlineStr"/>
+      <c r="F983" t="inlineStr"/>
+      <c r="G983" t="inlineStr"/>
+      <c r="H983" t="inlineStr"/>
+      <c r="I983" t="inlineStr"/>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>Title: Private Texas Hill Country Half-Day Wine Tour from Austin</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr"/>
+      <c r="C984" t="inlineStr"/>
+      <c r="D984" t="inlineStr"/>
+      <c r="E984" t="inlineStr"/>
+      <c r="F984" t="inlineStr"/>
+      <c r="G984" t="inlineStr"/>
+      <c r="H984" t="inlineStr"/>
+      <c r="I984" t="inlineStr"/>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>TotalReviews: 19</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr"/>
+      <c r="C985" t="inlineStr"/>
+      <c r="D985" t="inlineStr"/>
+      <c r="E985" t="inlineStr"/>
+      <c r="F985" t="inlineStr"/>
+      <c r="G985" t="inlineStr"/>
+      <c r="H985" t="inlineStr"/>
+      <c r="I985" t="inlineStr"/>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>Category: ['Wine and Beverage Tastings', 'Culinary Tours']</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr"/>
+      <c r="C986" t="inlineStr"/>
+      <c r="D986" t="inlineStr"/>
+      <c r="E986" t="inlineStr"/>
+      <c r="F986" t="inlineStr"/>
+      <c r="G986" t="inlineStr"/>
+      <c r="H986" t="inlineStr"/>
+      <c r="I986" t="inlineStr"/>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>PRODUCTCODE: 199613P1</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr"/>
+      <c r="C987" t="inlineStr"/>
+      <c r="D987" t="inlineStr"/>
+      <c r="E987" t="inlineStr"/>
+      <c r="F987" t="inlineStr"/>
+      <c r="G987" t="inlineStr"/>
+      <c r="H987" t="inlineStr"/>
+      <c r="I987" t="inlineStr"/>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>Summarized description: The Texas Hill Country Winery, Brewery &amp; Salt Lick BBQ Charter is the perfect option for solo travelers, couples, families, and small groups. Our driver-guides are experts in the area and locations we visit, assuring you the best possible experience. This charter is a great way to meet other locals and those also traveling to Austin.</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr"/>
+      <c r="C988" t="inlineStr"/>
+      <c r="D988" t="inlineStr"/>
+      <c r="E988" t="inlineStr"/>
+      <c r="F988" t="inlineStr"/>
+      <c r="G988" t="inlineStr"/>
+      <c r="H988" t="inlineStr"/>
+      <c r="I988" t="inlineStr"/>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>Title: Best of Texas Hill Country Wine, Beer &amp; BBQ Tour from Austin</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr"/>
+      <c r="C989" t="inlineStr"/>
+      <c r="D989" t="inlineStr"/>
+      <c r="E989" t="inlineStr"/>
+      <c r="F989" t="inlineStr"/>
+      <c r="G989" t="inlineStr"/>
+      <c r="H989" t="inlineStr"/>
+      <c r="I989" t="inlineStr"/>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>TotalReviews: 14</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr"/>
+      <c r="C990" t="inlineStr"/>
+      <c r="D990" t="inlineStr"/>
+      <c r="E990" t="inlineStr"/>
+      <c r="F990" t="inlineStr"/>
+      <c r="G990" t="inlineStr"/>
+      <c r="H990" t="inlineStr"/>
+      <c r="I990" t="inlineStr"/>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>Category: ['Wine and Beverage Tastings', 'Culinary Tours']</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr"/>
+      <c r="C991" t="inlineStr"/>
+      <c r="D991" t="inlineStr"/>
+      <c r="E991" t="inlineStr"/>
+      <c r="F991" t="inlineStr"/>
+      <c r="G991" t="inlineStr"/>
+      <c r="H991" t="inlineStr"/>
+      <c r="I991" t="inlineStr"/>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>PRODUCTCODE: 51066P9</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr"/>
+      <c r="C992" t="inlineStr"/>
+      <c r="D992" t="inlineStr"/>
+      <c r="E992" t="inlineStr"/>
+      <c r="F992" t="inlineStr"/>
+      <c r="G992" t="inlineStr"/>
+      <c r="H992" t="inlineStr"/>
+      <c r="I992" t="inlineStr"/>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>Summarized description: 3-hour barbecue and beer tour. Stop at one of Austin's many bars and restaurants. Take an open-air electric shuttle from your hotel or visitor's center.</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr"/>
+      <c r="C993" t="inlineStr"/>
+      <c r="D993" t="inlineStr"/>
+      <c r="E993" t="inlineStr"/>
+      <c r="F993" t="inlineStr"/>
+      <c r="G993" t="inlineStr"/>
+      <c r="H993" t="inlineStr"/>
+      <c r="I993" t="inlineStr"/>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>Title: Brew and Que Tour in Austin</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr"/>
+      <c r="C994" t="inlineStr"/>
+      <c r="D994" t="inlineStr"/>
+      <c r="E994" t="inlineStr"/>
+      <c r="F994" t="inlineStr"/>
+      <c r="G994" t="inlineStr"/>
+      <c r="H994" t="inlineStr"/>
+      <c r="I994" t="inlineStr"/>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>TotalReviews: 12</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr"/>
+      <c r="C995" t="inlineStr"/>
+      <c r="D995" t="inlineStr"/>
+      <c r="E995" t="inlineStr"/>
+      <c r="F995" t="inlineStr"/>
+      <c r="G995" t="inlineStr"/>
+      <c r="H995" t="inlineStr"/>
+      <c r="I995" t="inlineStr"/>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>Category: ['City Tours', 'Culinary Tours']</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr"/>
+      <c r="C996" t="inlineStr"/>
+      <c r="D996" t="inlineStr"/>
+      <c r="E996" t="inlineStr"/>
+      <c r="F996" t="inlineStr"/>
+      <c r="G996" t="inlineStr"/>
+      <c r="H996" t="inlineStr"/>
+      <c r="I996" t="inlineStr"/>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>PRODUCTCODE: 25815P7</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr"/>
+      <c r="C997" t="inlineStr"/>
+      <c r="D997" t="inlineStr"/>
+      <c r="E997" t="inlineStr"/>
+      <c r="F997" t="inlineStr"/>
+      <c r="G997" t="inlineStr"/>
+      <c r="H997" t="inlineStr"/>
+      <c r="I997" t="inlineStr"/>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>Summarized description: Get an insider's view of how olives are pressed and what makes olive oil "Extra Virgin" This tour is a short drive outside of Austin Texas. Topics include History of the Orchard, How olives were milled and pressed, Extra Virgin 101.</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr"/>
+      <c r="C998" t="inlineStr"/>
+      <c r="D998" t="inlineStr"/>
+      <c r="E998" t="inlineStr"/>
+      <c r="F998" t="inlineStr"/>
+      <c r="G998" t="inlineStr"/>
+      <c r="H998" t="inlineStr"/>
+      <c r="I998" t="inlineStr"/>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>Title: Texas Hill Country Olive Mill Tour &amp; Extra Virgin 101</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr"/>
+      <c r="C999" t="inlineStr"/>
+      <c r="D999" t="inlineStr"/>
+      <c r="E999" t="inlineStr"/>
+      <c r="F999" t="inlineStr"/>
+      <c r="G999" t="inlineStr"/>
+      <c r="H999" t="inlineStr"/>
+      <c r="I999" t="inlineStr"/>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>TotalReviews: 9</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr"/>
+      <c r="C1000" t="inlineStr"/>
+      <c r="D1000" t="inlineStr"/>
+      <c r="E1000" t="inlineStr"/>
+      <c r="F1000" t="inlineStr"/>
+      <c r="G1000" t="inlineStr"/>
+      <c r="H1000" t="inlineStr"/>
+      <c r="I1000" t="inlineStr"/>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>Category: ['Culinary Tours']</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr"/>
+      <c r="C1001" t="inlineStr"/>
+      <c r="D1001" t="inlineStr"/>
+      <c r="E1001" t="inlineStr"/>
+      <c r="F1001" t="inlineStr"/>
+      <c r="G1001" t="inlineStr"/>
+      <c r="H1001" t="inlineStr"/>
+      <c r="I1001" t="inlineStr"/>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>PRODUCTCODE: 199613P4</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr"/>
+      <c r="C1002" t="inlineStr"/>
+      <c r="D1002" t="inlineStr"/>
+      <c r="E1002" t="inlineStr"/>
+      <c r="F1002" t="inlineStr"/>
+      <c r="G1002" t="inlineStr"/>
+      <c r="H1002" t="inlineStr"/>
+      <c r="I1002" t="inlineStr"/>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>Summarized description: Texas Tipsy Tours’ experience includes wine tastings at top Texas Hill Country wineries. Stop at iconic Salt Lick BBQ and Cellars, plus time for shopping, dining and/or drinks in two charming hill country towns. This semi-private tour has a max capacity of 13, giving you a uniquely intimate experience.</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr"/>
+      <c r="C1003" t="inlineStr"/>
+      <c r="D1003" t="inlineStr"/>
+      <c r="E1003" t="inlineStr"/>
+      <c r="F1003" t="inlineStr"/>
+      <c r="G1003" t="inlineStr"/>
+      <c r="H1003" t="inlineStr"/>
+      <c r="I1003" t="inlineStr"/>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Title: Hill Country Wine Tour of Dripping Springs and Wimberley </t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr"/>
+      <c r="C1004" t="inlineStr"/>
+      <c r="D1004" t="inlineStr"/>
+      <c r="E1004" t="inlineStr"/>
+      <c r="F1004" t="inlineStr"/>
+      <c r="G1004" t="inlineStr"/>
+      <c r="H1004" t="inlineStr"/>
+      <c r="I1004" t="inlineStr"/>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>TotalReviews: 8</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr"/>
+      <c r="C1005" t="inlineStr"/>
+      <c r="D1005" t="inlineStr"/>
+      <c r="E1005" t="inlineStr"/>
+      <c r="F1005" t="inlineStr"/>
+      <c r="G1005" t="inlineStr"/>
+      <c r="H1005" t="inlineStr"/>
+      <c r="I1005" t="inlineStr"/>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>Category: ['Wine and Beverage Tastings', 'Culinary Tours']</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr"/>
+      <c r="C1006" t="inlineStr"/>
+      <c r="D1006" t="inlineStr"/>
+      <c r="E1006" t="inlineStr"/>
+      <c r="F1006" t="inlineStr"/>
+      <c r="G1006" t="inlineStr"/>
+      <c r="H1006" t="inlineStr"/>
+      <c r="I1006" t="inlineStr"/>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>PRODUCTCODE: 87115P52</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr"/>
+      <c r="C1007" t="inlineStr"/>
+      <c r="D1007" t="inlineStr"/>
+      <c r="E1007" t="inlineStr"/>
+      <c r="F1007" t="inlineStr"/>
+      <c r="G1007" t="inlineStr"/>
+      <c r="H1007" t="inlineStr"/>
+      <c r="I1007" t="inlineStr"/>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>Summarized description: Taste the best BBQ that Austin has to offer on our Austin Red River Street BBQ Food Walking Tour. Not only will you get to sample delicious barbecue, you will also witness many must-see places throughout The Red River Cultural District.</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr"/>
+      <c r="C1008" t="inlineStr"/>
+      <c r="D1008" t="inlineStr"/>
+      <c r="E1008" t="inlineStr"/>
+      <c r="F1008" t="inlineStr"/>
+      <c r="G1008" t="inlineStr"/>
+      <c r="H1008" t="inlineStr"/>
+      <c r="I1008" t="inlineStr"/>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>Title: Small Group Austin Red River Street BBQ Food Walking Tour</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr"/>
+      <c r="C1009" t="inlineStr"/>
+      <c r="D1009" t="inlineStr"/>
+      <c r="E1009" t="inlineStr"/>
+      <c r="F1009" t="inlineStr"/>
+      <c r="G1009" t="inlineStr"/>
+      <c r="H1009" t="inlineStr"/>
+      <c r="I1009" t="inlineStr"/>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>TotalReviews: 5</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr"/>
+      <c r="C1010" t="inlineStr"/>
+      <c r="D1010" t="inlineStr"/>
+      <c r="E1010" t="inlineStr"/>
+      <c r="F1010" t="inlineStr"/>
+      <c r="G1010" t="inlineStr"/>
+      <c r="H1010" t="inlineStr"/>
+      <c r="I1010" t="inlineStr"/>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>Category: ['Culinary Tours']</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr"/>
+      <c r="C1011" t="inlineStr"/>
+      <c r="D1011" t="inlineStr"/>
+      <c r="E1011" t="inlineStr"/>
+      <c r="F1011" t="inlineStr"/>
+      <c r="G1011" t="inlineStr"/>
+      <c r="H1011" t="inlineStr"/>
+      <c r="I1011" t="inlineStr"/>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>PRODUCTCODE: 19328P2</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr"/>
+      <c r="C1012" t="inlineStr"/>
+      <c r="D1012" t="inlineStr"/>
+      <c r="E1012" t="inlineStr"/>
+      <c r="F1012" t="inlineStr"/>
+      <c r="G1012" t="inlineStr"/>
+      <c r="H1012" t="inlineStr"/>
+      <c r="I1012" t="inlineStr"/>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>Summarized description: Texas has been named one of the best places for barbecue in the world. Lockhart is said to be the Barbecue Capital of the World. There are thousands of BBQ joints across the state.</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr"/>
+      <c r="C1013" t="inlineStr"/>
+      <c r="D1013" t="inlineStr"/>
+      <c r="E1013" t="inlineStr"/>
+      <c r="F1013" t="inlineStr"/>
+      <c r="G1013" t="inlineStr"/>
+      <c r="H1013" t="inlineStr"/>
+      <c r="I1013" t="inlineStr"/>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>Title: Austin Food Tour: Texas BBQ Trail</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr"/>
+      <c r="C1014" t="inlineStr"/>
+      <c r="D1014" t="inlineStr"/>
+      <c r="E1014" t="inlineStr"/>
+      <c r="F1014" t="inlineStr"/>
+      <c r="G1014" t="inlineStr"/>
+      <c r="H1014" t="inlineStr"/>
+      <c r="I1014" t="inlineStr"/>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>TotalReviews: 4</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr"/>
+      <c r="C1015" t="inlineStr"/>
+      <c r="D1015" t="inlineStr"/>
+      <c r="E1015" t="inlineStr"/>
+      <c r="F1015" t="inlineStr"/>
+      <c r="G1015" t="inlineStr"/>
+      <c r="H1015" t="inlineStr"/>
+      <c r="I1015" t="inlineStr"/>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>Category: ['Culinary Tours']</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr"/>
+      <c r="C1016" t="inlineStr"/>
+      <c r="D1016" t="inlineStr"/>
+      <c r="E1016" t="inlineStr"/>
+      <c r="F1016" t="inlineStr"/>
+      <c r="G1016" t="inlineStr"/>
+      <c r="H1016" t="inlineStr"/>
+      <c r="I1016" t="inlineStr"/>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>PRODUCTCODE: 201132P1</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr"/>
+      <c r="C1017" t="inlineStr"/>
+      <c r="D1017" t="inlineStr"/>
+      <c r="E1017" t="inlineStr"/>
+      <c r="F1017" t="inlineStr"/>
+      <c r="G1017" t="inlineStr"/>
+      <c r="H1017" t="inlineStr"/>
+      <c r="I1017" t="inlineStr"/>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>Summarized description: Enjoy throwback tunes while sipping on award winning Texas wines. Our motto Peace, Love, and Wine is definitely felt during your 5 hour tour through the beautiful hills of the Texas hill country.</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr"/>
+      <c r="C1018" t="inlineStr"/>
+      <c r="D1018" t="inlineStr"/>
+      <c r="E1018" t="inlineStr"/>
+      <c r="F1018" t="inlineStr"/>
+      <c r="G1018" t="inlineStr"/>
+      <c r="H1018" t="inlineStr"/>
+      <c r="I1018" t="inlineStr"/>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>Title: Retro Wine Tour in A Vintage VW Bus</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr"/>
+      <c r="C1019" t="inlineStr"/>
+      <c r="D1019" t="inlineStr"/>
+      <c r="E1019" t="inlineStr"/>
+      <c r="F1019" t="inlineStr"/>
+      <c r="G1019" t="inlineStr"/>
+      <c r="H1019" t="inlineStr"/>
+      <c r="I1019" t="inlineStr"/>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>TotalReviews: 4</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr"/>
+      <c r="C1020" t="inlineStr"/>
+      <c r="D1020" t="inlineStr"/>
+      <c r="E1020" t="inlineStr"/>
+      <c r="F1020" t="inlineStr"/>
+      <c r="G1020" t="inlineStr"/>
+      <c r="H1020" t="inlineStr"/>
+      <c r="I1020" t="inlineStr"/>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>Category: ['Wine and Beverage Tastings']</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr"/>
+      <c r="C1021" t="inlineStr"/>
+      <c r="D1021" t="inlineStr"/>
+      <c r="E1021" t="inlineStr"/>
+      <c r="F1021" t="inlineStr"/>
+      <c r="G1021" t="inlineStr"/>
+      <c r="H1021" t="inlineStr"/>
+      <c r="I1021" t="inlineStr"/>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>PRODUCTCODE: 199613P3</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr"/>
+      <c r="C1022" t="inlineStr"/>
+      <c r="D1022" t="inlineStr"/>
+      <c r="E1022" t="inlineStr"/>
+      <c r="F1022" t="inlineStr"/>
+      <c r="G1022" t="inlineStr"/>
+      <c r="H1022" t="inlineStr"/>
+      <c r="I1022" t="inlineStr"/>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>Summarized description: Texas Tipsy Tours offers a semi-private tour for mixed, small groups with pick-ups at your hotel in Downtown Austin. Visit three customer-favorite Driftwood wineries, as well as a stop at Salt Lick BBQ &amp; Cellars, an iconic Austin BBQ restaurant.</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr"/>
+      <c r="C1023" t="inlineStr"/>
+      <c r="D1023" t="inlineStr"/>
+      <c r="E1023" t="inlineStr"/>
+      <c r="F1023" t="inlineStr"/>
+      <c r="G1023" t="inlineStr"/>
+      <c r="H1023" t="inlineStr"/>
+      <c r="I1023" t="inlineStr"/>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Title: Hill Country Wine Tour and Salt Lick BBQ Tour from Austin </t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr"/>
+      <c r="C1024" t="inlineStr"/>
+      <c r="D1024" t="inlineStr"/>
+      <c r="E1024" t="inlineStr"/>
+      <c r="F1024" t="inlineStr"/>
+      <c r="G1024" t="inlineStr"/>
+      <c r="H1024" t="inlineStr"/>
+      <c r="I1024" t="inlineStr"/>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>TotalReviews: 4</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr"/>
+      <c r="C1025" t="inlineStr"/>
+      <c r="D1025" t="inlineStr"/>
+      <c r="E1025" t="inlineStr"/>
+      <c r="F1025" t="inlineStr"/>
+      <c r="G1025" t="inlineStr"/>
+      <c r="H1025" t="inlineStr"/>
+      <c r="I1025" t="inlineStr"/>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>Category: ['Wine and Beverage Tastings', 'Culinary Tours']</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr"/>
+      <c r="C1026" t="inlineStr"/>
+      <c r="D1026" t="inlineStr"/>
+      <c r="E1026" t="inlineStr"/>
+      <c r="F1026" t="inlineStr"/>
+      <c r="G1026" t="inlineStr"/>
+      <c r="H1026" t="inlineStr"/>
+      <c r="I1026" t="inlineStr"/>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>PRODUCTCODE: 327690P1</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr"/>
+      <c r="C1027" t="inlineStr"/>
+      <c r="D1027" t="inlineStr"/>
+      <c r="E1027" t="inlineStr"/>
+      <c r="F1027" t="inlineStr"/>
+      <c r="G1027" t="inlineStr"/>
+      <c r="H1027" t="inlineStr"/>
+      <c r="I1027" t="inlineStr"/>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>Summarized description: The Half Day Hill Country in Limousine wine tour is approximately 4-6 hours from pick up to drop off. You will tour 3 great Driftwood/Dripping Springs wineries where you will enjoy the absolute best wines.</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr"/>
+      <c r="C1028" t="inlineStr"/>
+      <c r="D1028" t="inlineStr"/>
+      <c r="E1028" t="inlineStr"/>
+      <c r="F1028" t="inlineStr"/>
+      <c r="G1028" t="inlineStr"/>
+      <c r="H1028" t="inlineStr"/>
+      <c r="I1028" t="inlineStr"/>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>Title: Half Day Wine Tour with Luxury Limousine in Austin</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr"/>
+      <c r="C1029" t="inlineStr"/>
+      <c r="D1029" t="inlineStr"/>
+      <c r="E1029" t="inlineStr"/>
+      <c r="F1029" t="inlineStr"/>
+      <c r="G1029" t="inlineStr"/>
+      <c r="H1029" t="inlineStr"/>
+      <c r="I1029" t="inlineStr"/>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>TotalReviews: 3</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr"/>
+      <c r="C1030" t="inlineStr"/>
+      <c r="D1030" t="inlineStr"/>
+      <c r="E1030" t="inlineStr"/>
+      <c r="F1030" t="inlineStr"/>
+      <c r="G1030" t="inlineStr"/>
+      <c r="H1030" t="inlineStr"/>
+      <c r="I1030" t="inlineStr"/>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>Category: ['Wine and Beverage Tastings', 'Scenic Tours']</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr"/>
+      <c r="C1031" t="inlineStr"/>
+      <c r="D1031" t="inlineStr"/>
+      <c r="E1031" t="inlineStr"/>
+      <c r="F1031" t="inlineStr"/>
+      <c r="G1031" t="inlineStr"/>
+      <c r="H1031" t="inlineStr"/>
+      <c r="I1031" t="inlineStr"/>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>PRODUCTCODE: 90519P11</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr"/>
+      <c r="C1032" t="inlineStr"/>
+      <c r="D1032" t="inlineStr"/>
+      <c r="E1032" t="inlineStr"/>
+      <c r="F1032" t="inlineStr"/>
+      <c r="G1032" t="inlineStr"/>
+      <c r="H1032" t="inlineStr"/>
+      <c r="I1032" t="inlineStr"/>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>Summarized description: The 290 Wine Shuttle costs $39.99 and stops at each of the locations on the route approximately every 10 minutes. You can't book a private bus to get this experience! Book your Austin to Fredericksburg Roundtrip Shuttle ticket today!!</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr"/>
+      <c r="C1033" t="inlineStr"/>
+      <c r="D1033" t="inlineStr"/>
+      <c r="E1033" t="inlineStr"/>
+      <c r="F1033" t="inlineStr"/>
+      <c r="G1033" t="inlineStr"/>
+      <c r="H1033" t="inlineStr"/>
+      <c r="I1033" t="inlineStr"/>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>Title: Austin to Fredericksburg Round Trip Transportation</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr"/>
+      <c r="C1034" t="inlineStr"/>
+      <c r="D1034" t="inlineStr"/>
+      <c r="E1034" t="inlineStr"/>
+      <c r="F1034" t="inlineStr"/>
+      <c r="G1034" t="inlineStr"/>
+      <c r="H1034" t="inlineStr"/>
+      <c r="I1034" t="inlineStr"/>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>TotalReviews: 3</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr"/>
+      <c r="C1035" t="inlineStr"/>
+      <c r="D1035" t="inlineStr"/>
+      <c r="E1035" t="inlineStr"/>
+      <c r="F1035" t="inlineStr"/>
+      <c r="G1035" t="inlineStr"/>
+      <c r="H1035" t="inlineStr"/>
+      <c r="I1035" t="inlineStr"/>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>Category: ['Transportation &amp; Travel Services']</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr"/>
+      <c r="C1036" t="inlineStr"/>
+      <c r="D1036" t="inlineStr"/>
+      <c r="E1036" t="inlineStr"/>
+      <c r="F1036" t="inlineStr"/>
+      <c r="G1036" t="inlineStr"/>
+      <c r="H1036" t="inlineStr"/>
+      <c r="I1036" t="inlineStr"/>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>PRODUCTCODE: 324527P1</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr"/>
+      <c r="C1037" t="inlineStr"/>
+      <c r="D1037" t="inlineStr"/>
+      <c r="E1037" t="inlineStr"/>
+      <c r="F1037" t="inlineStr"/>
+      <c r="G1037" t="inlineStr"/>
+      <c r="H1037" t="inlineStr"/>
+      <c r="I1037" t="inlineStr"/>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>Summarized description: Enjoy a personalized Tour of Austin and surrounding Hill Country with up to 14 guests. We have some great spots we know you'll love or we can plan a unique trip just for you. Great for a bachelor/ettes party’s or can be a site seeing family trip!</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr"/>
+      <c r="C1038" t="inlineStr"/>
+      <c r="D1038" t="inlineStr"/>
+      <c r="E1038" t="inlineStr"/>
+      <c r="F1038" t="inlineStr"/>
+      <c r="G1038" t="inlineStr"/>
+      <c r="H1038" t="inlineStr"/>
+      <c r="I1038" t="inlineStr"/>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>Title: Personalized Tour of Austin and Surrounding Hill Country</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr"/>
+      <c r="C1039" t="inlineStr"/>
+      <c r="D1039" t="inlineStr"/>
+      <c r="E1039" t="inlineStr"/>
+      <c r="F1039" t="inlineStr"/>
+      <c r="G1039" t="inlineStr"/>
+      <c r="H1039" t="inlineStr"/>
+      <c r="I1039" t="inlineStr"/>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>TotalReviews: 2</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr"/>
+      <c r="C1040" t="inlineStr"/>
+      <c r="D1040" t="inlineStr"/>
+      <c r="E1040" t="inlineStr"/>
+      <c r="F1040" t="inlineStr"/>
+      <c r="G1040" t="inlineStr"/>
+      <c r="H1040" t="inlineStr"/>
+      <c r="I1040" t="inlineStr"/>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>Category: ['City Tours', 'Scenic Tours']</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr"/>
+      <c r="C1041" t="inlineStr"/>
+      <c r="D1041" t="inlineStr"/>
+      <c r="E1041" t="inlineStr"/>
+      <c r="F1041" t="inlineStr"/>
+      <c r="G1041" t="inlineStr"/>
+      <c r="H1041" t="inlineStr"/>
+      <c r="I1041" t="inlineStr"/>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>PRODUCTCODE: 288955P2</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr"/>
+      <c r="C1042" t="inlineStr"/>
+      <c r="D1042" t="inlineStr"/>
+      <c r="E1042" t="inlineStr"/>
+      <c r="F1042" t="inlineStr"/>
+      <c r="G1042" t="inlineStr"/>
+      <c r="H1042" t="inlineStr"/>
+      <c r="I1042" t="inlineStr"/>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>Summarized description:  Shuttle bus takes group on the Central Texas Beer &amp; Wine Trail. Stops include Dancing Bee Winery, Bold Republic Brewing Company and 3 Texans Winery. Plan for a 1-hour stop at each location.</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr"/>
+      <c r="C1043" t="inlineStr"/>
+      <c r="D1043" t="inlineStr"/>
+      <c r="E1043" t="inlineStr"/>
+      <c r="F1043" t="inlineStr"/>
+      <c r="G1043" t="inlineStr"/>
+      <c r="H1043" t="inlineStr"/>
+      <c r="I1043" t="inlineStr"/>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>Title: Beer &amp; Wine Trail Friday (4pm-8pm)</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr"/>
+      <c r="C1044" t="inlineStr"/>
+      <c r="D1044" t="inlineStr"/>
+      <c r="E1044" t="inlineStr"/>
+      <c r="F1044" t="inlineStr"/>
+      <c r="G1044" t="inlineStr"/>
+      <c r="H1044" t="inlineStr"/>
+      <c r="I1044" t="inlineStr"/>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>TotalReviews: 2</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr"/>
+      <c r="C1045" t="inlineStr"/>
+      <c r="D1045" t="inlineStr"/>
+      <c r="E1045" t="inlineStr"/>
+      <c r="F1045" t="inlineStr"/>
+      <c r="G1045" t="inlineStr"/>
+      <c r="H1045" t="inlineStr"/>
+      <c r="I1045" t="inlineStr"/>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>Category: ['Wine and Beverage Tastings']</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr"/>
+      <c r="C1046" t="inlineStr"/>
+      <c r="D1046" t="inlineStr"/>
+      <c r="E1046" t="inlineStr"/>
+      <c r="F1046" t="inlineStr"/>
+      <c r="G1046" t="inlineStr"/>
+      <c r="H1046" t="inlineStr"/>
+      <c r="I1046" t="inlineStr"/>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>PRODUCTCODE: 348643P1</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr"/>
+      <c r="C1047" t="inlineStr"/>
+      <c r="D1047" t="inlineStr"/>
+      <c r="E1047" t="inlineStr"/>
+      <c r="F1047" t="inlineStr"/>
+      <c r="G1047" t="inlineStr"/>
+      <c r="H1047" t="inlineStr"/>
+      <c r="I1047" t="inlineStr"/>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>Summarized description: We are the company to get you out of Austin for the day! We take you on breathtaking views of the amazing Texas Hill Country. You will be guided by one of our very experienced hosts who will pick you up in the downtown Austin area.</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr"/>
+      <c r="C1048" t="inlineStr"/>
+      <c r="D1048" t="inlineStr"/>
+      <c r="E1048" t="inlineStr"/>
+      <c r="F1048" t="inlineStr"/>
+      <c r="G1048" t="inlineStr"/>
+      <c r="H1048" t="inlineStr"/>
+      <c r="I1048" t="inlineStr"/>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>Title: Escape the day from Austin to Fredericksburg, Luchenbach</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr"/>
+      <c r="C1049" t="inlineStr"/>
+      <c r="D1049" t="inlineStr"/>
+      <c r="E1049" t="inlineStr"/>
+      <c r="F1049" t="inlineStr"/>
+      <c r="G1049" t="inlineStr"/>
+      <c r="H1049" t="inlineStr"/>
+      <c r="I1049" t="inlineStr"/>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>TotalReviews: 1</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr"/>
+      <c r="C1050" t="inlineStr"/>
+      <c r="D1050" t="inlineStr"/>
+      <c r="E1050" t="inlineStr"/>
+      <c r="F1050" t="inlineStr"/>
+      <c r="G1050" t="inlineStr"/>
+      <c r="H1050" t="inlineStr"/>
+      <c r="I1050" t="inlineStr"/>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>Category: ['City Tours', 'Scenic Tours', 'Cultural Tours']</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr"/>
+      <c r="C1051" t="inlineStr"/>
+      <c r="D1051" t="inlineStr"/>
+      <c r="E1051" t="inlineStr"/>
+      <c r="F1051" t="inlineStr"/>
+      <c r="G1051" t="inlineStr"/>
+      <c r="H1051" t="inlineStr"/>
+      <c r="I1051" t="inlineStr"/>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>PRODUCTCODE: 288955P8</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr"/>
+      <c r="C1052" t="inlineStr"/>
+      <c r="D1052" t="inlineStr"/>
+      <c r="E1052" t="inlineStr"/>
+      <c r="F1052" t="inlineStr"/>
+      <c r="G1052" t="inlineStr"/>
+      <c r="H1052" t="inlineStr"/>
+      <c r="I1052" t="inlineStr"/>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>Summarized description:  Shuttle bus takes group on Central Texas Wine Trail. Stops include Dancing Bee Winery, Axis Winery and 3 Texans Winery. Plan for a 1-hour stop at each location as venue staff hosts you.</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr"/>
+      <c r="C1053" t="inlineStr"/>
+      <c r="D1053" t="inlineStr"/>
+      <c r="E1053" t="inlineStr"/>
+      <c r="F1053" t="inlineStr"/>
+      <c r="G1053" t="inlineStr"/>
+      <c r="H1053" t="inlineStr"/>
+      <c r="I1053" t="inlineStr"/>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>Title: Wine Trail Tour Sunday (2pm-6pm)</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr"/>
+      <c r="C1054" t="inlineStr"/>
+      <c r="D1054" t="inlineStr"/>
+      <c r="E1054" t="inlineStr"/>
+      <c r="F1054" t="inlineStr"/>
+      <c r="G1054" t="inlineStr"/>
+      <c r="H1054" t="inlineStr"/>
+      <c r="I1054" t="inlineStr"/>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>TotalReviews: 1</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr"/>
+      <c r="C1055" t="inlineStr"/>
+      <c r="D1055" t="inlineStr"/>
+      <c r="E1055" t="inlineStr"/>
+      <c r="F1055" t="inlineStr"/>
+      <c r="G1055" t="inlineStr"/>
+      <c r="H1055" t="inlineStr"/>
+      <c r="I1055" t="inlineStr"/>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>Category: ['Wine and Beverage Tastings']</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr"/>
+      <c r="C1056" t="inlineStr"/>
+      <c r="D1056" t="inlineStr"/>
+      <c r="E1056" t="inlineStr"/>
+      <c r="F1056" t="inlineStr"/>
+      <c r="G1056" t="inlineStr"/>
+      <c r="H1056" t="inlineStr"/>
+      <c r="I1056" t="inlineStr"/>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>PRODUCTCODE: 288955P3</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr"/>
+      <c r="C1057" t="inlineStr"/>
+      <c r="D1057" t="inlineStr"/>
+      <c r="E1057" t="inlineStr"/>
+      <c r="F1057" t="inlineStr"/>
+      <c r="G1057" t="inlineStr"/>
+      <c r="H1057" t="inlineStr"/>
+      <c r="I1057" t="inlineStr"/>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>Summarized description:  Shuttle bus takes group on the Central Texas Beer &amp; Wine Trail. Stops include Dancing Bee Winery, Bold Republic Brewing Company and 3 Texans Winery. Plan for a 1-hour stop at each location.</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr"/>
+      <c r="C1058" t="inlineStr"/>
+      <c r="D1058" t="inlineStr"/>
+      <c r="E1058" t="inlineStr"/>
+      <c r="F1058" t="inlineStr"/>
+      <c r="G1058" t="inlineStr"/>
+      <c r="H1058" t="inlineStr"/>
+      <c r="I1058" t="inlineStr"/>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>Title: Wine &amp; Beer Trail Saturday (3pm-7pm)</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr"/>
+      <c r="C1059" t="inlineStr"/>
+      <c r="D1059" t="inlineStr"/>
+      <c r="E1059" t="inlineStr"/>
+      <c r="F1059" t="inlineStr"/>
+      <c r="G1059" t="inlineStr"/>
+      <c r="H1059" t="inlineStr"/>
+      <c r="I1059" t="inlineStr"/>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>TotalReviews: 1</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr"/>
+      <c r="C1060" t="inlineStr"/>
+      <c r="D1060" t="inlineStr"/>
+      <c r="E1060" t="inlineStr"/>
+      <c r="F1060" t="inlineStr"/>
+      <c r="G1060" t="inlineStr"/>
+      <c r="H1060" t="inlineStr"/>
+      <c r="I1060" t="inlineStr"/>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>Category: ['Wine and Beverage Tastings']</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr"/>
+      <c r="C1061" t="inlineStr"/>
+      <c r="D1061" t="inlineStr"/>
+      <c r="E1061" t="inlineStr"/>
+      <c r="F1061" t="inlineStr"/>
+      <c r="G1061" t="inlineStr"/>
+      <c r="H1061" t="inlineStr"/>
+      <c r="I1061" t="inlineStr"/>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>PRODUCTCODE: 90519P16</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr"/>
+      <c r="C1062" t="inlineStr"/>
+      <c r="D1062" t="inlineStr"/>
+      <c r="E1062" t="inlineStr"/>
+      <c r="F1062" t="inlineStr"/>
+      <c r="G1062" t="inlineStr"/>
+      <c r="H1062" t="inlineStr"/>
+      <c r="I1062" t="inlineStr"/>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>Summarized description: Tour Austin is partnering with the 290 Wine Shuttle so Austin residents can experience the best of Fredericksburg for a day without the need to drive. The shuttle stops at each of the locations on the route approximately every 10 minutes. Book your shuttle rides today!!</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr"/>
+      <c r="C1063" t="inlineStr"/>
+      <c r="D1063" t="inlineStr"/>
+      <c r="E1063" t="inlineStr"/>
+      <c r="F1063" t="inlineStr"/>
+      <c r="G1063" t="inlineStr"/>
+      <c r="H1063" t="inlineStr"/>
+      <c r="I1063" t="inlineStr"/>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>Title: 290 Wine Shuttle Austin Connection</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr"/>
+      <c r="C1064" t="inlineStr"/>
+      <c r="D1064" t="inlineStr"/>
+      <c r="E1064" t="inlineStr"/>
+      <c r="F1064" t="inlineStr"/>
+      <c r="G1064" t="inlineStr"/>
+      <c r="H1064" t="inlineStr"/>
+      <c r="I1064" t="inlineStr"/>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>TotalReviews: 1</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr"/>
+      <c r="C1065" t="inlineStr"/>
+      <c r="D1065" t="inlineStr"/>
+      <c r="E1065" t="inlineStr"/>
+      <c r="F1065" t="inlineStr"/>
+      <c r="G1065" t="inlineStr"/>
+      <c r="H1065" t="inlineStr"/>
+      <c r="I1065" t="inlineStr"/>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>Category: ['Wine and Beverage Tastings', 'Culinary Tours']</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr"/>
+      <c r="C1066" t="inlineStr"/>
+      <c r="D1066" t="inlineStr"/>
+      <c r="E1066" t="inlineStr"/>
+      <c r="F1066" t="inlineStr"/>
+      <c r="G1066" t="inlineStr"/>
+      <c r="H1066" t="inlineStr"/>
+      <c r="I1066" t="inlineStr"/>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>PRODUCTCODE: 251722P1</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr"/>
+      <c r="C1067" t="inlineStr"/>
+      <c r="D1067" t="inlineStr"/>
+      <c r="E1067" t="inlineStr"/>
+      <c r="F1067" t="inlineStr"/>
+      <c r="G1067" t="inlineStr"/>
+      <c r="H1067" t="inlineStr"/>
+      <c r="I1067" t="inlineStr"/>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>Summarized description: Explore some of Texas' most popular wineries and learn about the wine making process. Taste the flavors of Texas at the Austin's most famous BBQ joint. Enjoy at least 45 minutes at each stop.</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr"/>
+      <c r="C1068" t="inlineStr"/>
+      <c r="D1068" t="inlineStr"/>
+      <c r="E1068" t="inlineStr"/>
+      <c r="F1068" t="inlineStr"/>
+      <c r="G1068" t="inlineStr"/>
+      <c r="H1068" t="inlineStr"/>
+      <c r="I1068" t="inlineStr"/>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>Title:  Salt Lick BBQ and Winery Shuttle Tour</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr"/>
+      <c r="C1069" t="inlineStr"/>
+      <c r="D1069" t="inlineStr"/>
+      <c r="E1069" t="inlineStr"/>
+      <c r="F1069" t="inlineStr"/>
+      <c r="G1069" t="inlineStr"/>
+      <c r="H1069" t="inlineStr"/>
+      <c r="I1069" t="inlineStr"/>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>TotalReviews: 0</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr"/>
+      <c r="C1070" t="inlineStr"/>
+      <c r="D1070" t="inlineStr"/>
+      <c r="E1070" t="inlineStr"/>
+      <c r="F1070" t="inlineStr"/>
+      <c r="G1070" t="inlineStr"/>
+      <c r="H1070" t="inlineStr"/>
+      <c r="I1070" t="inlineStr"/>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>Category: ['Wine and Beverage Tastings', 'Culinary Tours']</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr"/>
+      <c r="C1071" t="inlineStr"/>
+      <c r="D1071" t="inlineStr"/>
+      <c r="E1071" t="inlineStr"/>
+      <c r="F1071" t="inlineStr"/>
+      <c r="G1071" t="inlineStr"/>
+      <c r="H1071" t="inlineStr"/>
+      <c r="I1071" t="inlineStr"/>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>PRODUCTCODE: 199613P5</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr"/>
+      <c r="C1072" t="inlineStr"/>
+      <c r="D1072" t="inlineStr"/>
+      <c r="E1072" t="inlineStr"/>
+      <c r="F1072" t="inlineStr"/>
+      <c r="G1072" t="inlineStr"/>
+      <c r="H1072" t="inlineStr"/>
+      <c r="I1072" t="inlineStr"/>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>Summarized description: Texas Tipsy Tours’ experience includes wine tastings at top Texas Hill Country wineries and a stop at iconic Salt Lick BBQ and Cellars. We will pick up and drop off at your chosen location inside Austin city limits.</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr"/>
+      <c r="C1073" t="inlineStr"/>
+      <c r="D1073" t="inlineStr"/>
+      <c r="E1073" t="inlineStr"/>
+      <c r="F1073" t="inlineStr"/>
+      <c r="G1073" t="inlineStr"/>
+      <c r="H1073" t="inlineStr"/>
+      <c r="I1073" t="inlineStr"/>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>Title: Private Driftwood Wine and BBQ Tour from Austin</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr"/>
+      <c r="C1074" t="inlineStr"/>
+      <c r="D1074" t="inlineStr"/>
+      <c r="E1074" t="inlineStr"/>
+      <c r="F1074" t="inlineStr"/>
+      <c r="G1074" t="inlineStr"/>
+      <c r="H1074" t="inlineStr"/>
+      <c r="I1074" t="inlineStr"/>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>TotalReviews: 0</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr"/>
+      <c r="C1075" t="inlineStr"/>
+      <c r="D1075" t="inlineStr"/>
+      <c r="E1075" t="inlineStr"/>
+      <c r="F1075" t="inlineStr"/>
+      <c r="G1075" t="inlineStr"/>
+      <c r="H1075" t="inlineStr"/>
+      <c r="I1075" t="inlineStr"/>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>Category: ['Wine and Beverage Tastings', 'Culinary Tours']</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr"/>
+      <c r="C1076" t="inlineStr"/>
+      <c r="D1076" t="inlineStr"/>
+      <c r="E1076" t="inlineStr"/>
+      <c r="F1076" t="inlineStr"/>
+      <c r="G1076" t="inlineStr"/>
+      <c r="H1076" t="inlineStr"/>
+      <c r="I1076" t="inlineStr"/>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>PRODUCTCODE: 90519P15</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr"/>
+      <c r="C1077" t="inlineStr"/>
+      <c r="D1077" t="inlineStr"/>
+      <c r="E1077" t="inlineStr"/>
+      <c r="F1077" t="inlineStr"/>
+      <c r="G1077" t="inlineStr"/>
+      <c r="H1077" t="inlineStr"/>
+      <c r="I1077" t="inlineStr"/>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>Summarized description: Tour Austin is partnering with the 290 Wine Shuttle so Austin residents can experience the best of Fredericksburg for a day without the need to drive. The shuttle stops at each of the locations on the route approximately every 10 minutes. Book your shuttle rides today!!</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr"/>
+      <c r="C1078" t="inlineStr"/>
+      <c r="D1078" t="inlineStr"/>
+      <c r="E1078" t="inlineStr"/>
+      <c r="F1078" t="inlineStr"/>
+      <c r="G1078" t="inlineStr"/>
+      <c r="H1078" t="inlineStr"/>
+      <c r="I1078" t="inlineStr"/>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>Title: 290 Wine Shuttle Austin Connection</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr"/>
+      <c r="C1079" t="inlineStr"/>
+      <c r="D1079" t="inlineStr"/>
+      <c r="E1079" t="inlineStr"/>
+      <c r="F1079" t="inlineStr"/>
+      <c r="G1079" t="inlineStr"/>
+      <c r="H1079" t="inlineStr"/>
+      <c r="I1079" t="inlineStr"/>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>TotalReviews: 0</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr"/>
+      <c r="C1080" t="inlineStr"/>
+      <c r="D1080" t="inlineStr"/>
+      <c r="E1080" t="inlineStr"/>
+      <c r="F1080" t="inlineStr"/>
+      <c r="G1080" t="inlineStr"/>
+      <c r="H1080" t="inlineStr"/>
+      <c r="I1080" t="inlineStr"/>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>Category: ['Wine and Beverage Tastings']</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr"/>
+      <c r="C1081" t="inlineStr"/>
+      <c r="D1081" t="inlineStr"/>
+      <c r="E1081" t="inlineStr"/>
+      <c r="F1081" t="inlineStr"/>
+      <c r="G1081" t="inlineStr"/>
+      <c r="H1081" t="inlineStr"/>
+      <c r="I1081" t="inlineStr"/>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>PRODUCTCODE: 320728P2775</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr"/>
+      <c r="C1082" t="inlineStr"/>
+      <c r="D1082" t="inlineStr"/>
+      <c r="E1082" t="inlineStr"/>
+      <c r="F1082" t="inlineStr"/>
+      <c r="G1082" t="inlineStr"/>
+      <c r="H1082" t="inlineStr"/>
+      <c r="I1082" t="inlineStr"/>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>Summarized description: Expert sommeliers and winemakers will guide you through tastings of exceptional wines, sharing their deep knowledge and passion for winemaking. Don't miss the opportunity to create lasting memories on this Half-Day Private Texas Hill Country Wine Tour.</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr"/>
+      <c r="C1083" t="inlineStr"/>
+      <c r="D1083" t="inlineStr"/>
+      <c r="E1083" t="inlineStr"/>
+      <c r="F1083" t="inlineStr"/>
+      <c r="G1083" t="inlineStr"/>
+      <c r="H1083" t="inlineStr"/>
+      <c r="I1083" t="inlineStr"/>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>Title: Half-Day Private Texas Hill Country Wine Tour from Austin</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr"/>
+      <c r="C1084" t="inlineStr"/>
+      <c r="D1084" t="inlineStr"/>
+      <c r="E1084" t="inlineStr"/>
+      <c r="F1084" t="inlineStr"/>
+      <c r="G1084" t="inlineStr"/>
+      <c r="H1084" t="inlineStr"/>
+      <c r="I1084" t="inlineStr"/>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>TotalReviews: 0</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr"/>
+      <c r="C1085" t="inlineStr"/>
+      <c r="D1085" t="inlineStr"/>
+      <c r="E1085" t="inlineStr"/>
+      <c r="F1085" t="inlineStr"/>
+      <c r="G1085" t="inlineStr"/>
+      <c r="H1085" t="inlineStr"/>
+      <c r="I1085" t="inlineStr"/>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>Category: ['Wine and Beverage Tastings', 'Culinary Tours']</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr"/>
+      <c r="C1086" t="inlineStr"/>
+      <c r="D1086" t="inlineStr"/>
+      <c r="E1086" t="inlineStr"/>
+      <c r="F1086" t="inlineStr"/>
+      <c r="G1086" t="inlineStr"/>
+      <c r="H1086" t="inlineStr"/>
+      <c r="I1086" t="inlineStr"/>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>PRODUCTCODE: 454873P1</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr"/>
+      <c r="C1087" t="inlineStr"/>
+      <c r="D1087" t="inlineStr"/>
+      <c r="E1087" t="inlineStr"/>
+      <c r="F1087" t="inlineStr"/>
+      <c r="G1087" t="inlineStr"/>
+      <c r="H1087" t="inlineStr"/>
+      <c r="I1087" t="inlineStr"/>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>Summarized description: The Brewery 5K Running Series includes a free beer and swag. The Bullock Texas State History Museum offers a self guided tour of the city's history. Terry Black's BBQ is one of Austin's most famous BBQ joints.</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr"/>
+      <c r="C1088" t="inlineStr"/>
+      <c r="D1088" t="inlineStr"/>
+      <c r="E1088" t="inlineStr"/>
+      <c r="F1088" t="inlineStr"/>
+      <c r="G1088" t="inlineStr"/>
+      <c r="H1088" t="inlineStr"/>
+      <c r="I1088" t="inlineStr"/>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Title: Brewery 5K Fun Run, BBQ, and Texas History Museum in Austin </t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr"/>
+      <c r="C1089" t="inlineStr"/>
+      <c r="D1089" t="inlineStr"/>
+      <c r="E1089" t="inlineStr"/>
+      <c r="F1089" t="inlineStr"/>
+      <c r="G1089" t="inlineStr"/>
+      <c r="H1089" t="inlineStr"/>
+      <c r="I1089" t="inlineStr"/>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>TotalReviews: 0</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr"/>
+      <c r="C1090" t="inlineStr"/>
+      <c r="D1090" t="inlineStr"/>
+      <c r="E1090" t="inlineStr"/>
+      <c r="F1090" t="inlineStr"/>
+      <c r="G1090" t="inlineStr"/>
+      <c r="H1090" t="inlineStr"/>
+      <c r="I1090" t="inlineStr"/>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>Category: ['Entertainment', 'Scenic Tours']</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr"/>
+      <c r="C1091" t="inlineStr"/>
+      <c r="D1091" t="inlineStr"/>
+      <c r="E1091" t="inlineStr"/>
+      <c r="F1091" t="inlineStr"/>
+      <c r="G1091" t="inlineStr"/>
+      <c r="H1091" t="inlineStr"/>
+      <c r="I1091" t="inlineStr"/>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>PRODUCTCODE: 87887P7</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr"/>
+      <c r="C1092" t="inlineStr"/>
+      <c r="D1092" t="inlineStr"/>
+      <c r="E1092" t="inlineStr"/>
+      <c r="F1092" t="inlineStr"/>
+      <c r="G1092" t="inlineStr"/>
+      <c r="H1092" t="inlineStr"/>
+      <c r="I1092" t="inlineStr"/>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>Summarized description: Enjoy traveling to local Austinite favorites in a private limousine. Visit distilleries that show you how the process works behind the scenes. Get a sampling of those you think are your favorites.</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr"/>
+      <c r="C1093" t="inlineStr"/>
+      <c r="D1093" t="inlineStr"/>
+      <c r="E1093" t="inlineStr"/>
+      <c r="F1093" t="inlineStr"/>
+      <c r="G1093" t="inlineStr"/>
+      <c r="H1093" t="inlineStr"/>
+      <c r="I1093" t="inlineStr"/>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>Title: Customizable Austin Distillery and Brewery Tour</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr"/>
+      <c r="C1094" t="inlineStr"/>
+      <c r="D1094" t="inlineStr"/>
+      <c r="E1094" t="inlineStr"/>
+      <c r="F1094" t="inlineStr"/>
+      <c r="G1094" t="inlineStr"/>
+      <c r="H1094" t="inlineStr"/>
+      <c r="I1094" t="inlineStr"/>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>TotalReviews: 0</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr"/>
+      <c r="C1095" t="inlineStr"/>
+      <c r="D1095" t="inlineStr"/>
+      <c r="E1095" t="inlineStr"/>
+      <c r="F1095" t="inlineStr"/>
+      <c r="G1095" t="inlineStr"/>
+      <c r="H1095" t="inlineStr"/>
+      <c r="I1095" t="inlineStr"/>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>Category: ['Wine and Beverage Tastings']</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr"/>
+      <c r="C1096" t="inlineStr"/>
+      <c r="D1096" t="inlineStr"/>
+      <c r="E1096" t="inlineStr"/>
+      <c r="F1096" t="inlineStr"/>
+      <c r="G1096" t="inlineStr"/>
+      <c r="H1096" t="inlineStr"/>
+      <c r="I1096" t="inlineStr"/>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>PRODUCTCODE: 263756P1</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr"/>
+      <c r="C1097" t="inlineStr"/>
+      <c r="D1097" t="inlineStr"/>
+      <c r="E1097" t="inlineStr"/>
+      <c r="F1097" t="inlineStr"/>
+      <c r="G1097" t="inlineStr"/>
+      <c r="H1097" t="inlineStr"/>
+      <c r="I1097" t="inlineStr"/>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>Summarized description: Professional guide who knows Austin and it's beer. Behind the scenes facility tour at one brewery. Hang with locals, eat at an Austin food truck. Visit 3 different breweries in one day.</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr"/>
+      <c r="C1098" t="inlineStr"/>
+      <c r="D1098" t="inlineStr"/>
+      <c r="E1098" t="inlineStr"/>
+      <c r="F1098" t="inlineStr"/>
+      <c r="G1098" t="inlineStr"/>
+      <c r="H1098" t="inlineStr"/>
+      <c r="I1098" t="inlineStr"/>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>Title: Half-Day Brewery and Craft Beer Tour in Austin with Tastings</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr"/>
+      <c r="C1099" t="inlineStr"/>
+      <c r="D1099" t="inlineStr"/>
+      <c r="E1099" t="inlineStr"/>
+      <c r="F1099" t="inlineStr"/>
+      <c r="G1099" t="inlineStr"/>
+      <c r="H1099" t="inlineStr"/>
+      <c r="I1099" t="inlineStr"/>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>TotalReviews: 0</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr"/>
+      <c r="C1100" t="inlineStr"/>
+      <c r="D1100" t="inlineStr"/>
+      <c r="E1100" t="inlineStr"/>
+      <c r="F1100" t="inlineStr"/>
+      <c r="G1100" t="inlineStr"/>
+      <c r="H1100" t="inlineStr"/>
+      <c r="I1100" t="inlineStr"/>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>Category: ['Cultural Tours', 'Dining Experiences']</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr"/>
+      <c r="C1101" t="inlineStr"/>
+      <c r="D1101" t="inlineStr"/>
+      <c r="E1101" t="inlineStr"/>
+      <c r="F1101" t="inlineStr"/>
+      <c r="G1101" t="inlineStr"/>
+      <c r="H1101" t="inlineStr"/>
+      <c r="I1101" t="inlineStr"/>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>PRODUCTCODE: 87115P25</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr"/>
+      <c r="C1102" t="inlineStr"/>
+      <c r="D1102" t="inlineStr"/>
+      <c r="E1102" t="inlineStr"/>
+      <c r="F1102" t="inlineStr"/>
+      <c r="G1102" t="inlineStr"/>
+      <c r="H1102" t="inlineStr"/>
+      <c r="I1102" t="inlineStr"/>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>Summarized description: See Sight Tours are Austin’s best small group tours (max. 7 guests). Enjoy the top attractions and visitor experiences while avoiding long lines and wait times. All attraction admission fees are included along with complimentary hotel pick up and drop off.</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr"/>
+      <c r="C1103" t="inlineStr"/>
+      <c r="D1103" t="inlineStr"/>
+      <c r="E1103" t="inlineStr"/>
+      <c r="F1103" t="inlineStr"/>
+      <c r="G1103" t="inlineStr"/>
+      <c r="H1103" t="inlineStr"/>
+      <c r="I1103" t="inlineStr"/>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>Title: Guided Tour of Austin's Highlights</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr"/>
+      <c r="C1104" t="inlineStr"/>
+      <c r="D1104" t="inlineStr"/>
+      <c r="E1104" t="inlineStr"/>
+      <c r="F1104" t="inlineStr"/>
+      <c r="G1104" t="inlineStr"/>
+      <c r="H1104" t="inlineStr"/>
+      <c r="I1104" t="inlineStr"/>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>TotalReviews: 0</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr"/>
+      <c r="C1105" t="inlineStr"/>
+      <c r="D1105" t="inlineStr"/>
+      <c r="E1105" t="inlineStr"/>
+      <c r="F1105" t="inlineStr"/>
+      <c r="G1105" t="inlineStr"/>
+      <c r="H1105" t="inlineStr"/>
+      <c r="I1105" t="inlineStr"/>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>Category: ['City Tours']</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr"/>
+      <c r="C1106" t="inlineStr"/>
+      <c r="D1106" t="inlineStr"/>
+      <c r="E1106" t="inlineStr"/>
+      <c r="F1106" t="inlineStr"/>
+      <c r="G1106" t="inlineStr"/>
+      <c r="H1106" t="inlineStr"/>
+      <c r="I1106" t="inlineStr"/>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>PRODUCTCODE: 260194P1</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr"/>
+      <c r="C1107" t="inlineStr"/>
+      <c r="D1107" t="inlineStr"/>
+      <c r="E1107" t="inlineStr"/>
+      <c r="F1107" t="inlineStr"/>
+      <c r="G1107" t="inlineStr"/>
+      <c r="H1107" t="inlineStr"/>
+      <c r="I1107" t="inlineStr"/>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>Summarized description: Tour the historic German settlement in the exquisite Texas Hill Country. Ride VIP on a Deluxe Motor Coach with reclining seats and extra legroom, perfect for napping.</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr"/>
+      <c r="C1108" t="inlineStr"/>
+      <c r="D1108" t="inlineStr"/>
+      <c r="E1108" t="inlineStr"/>
+      <c r="F1108" t="inlineStr"/>
+      <c r="G1108" t="inlineStr"/>
+      <c r="H1108" t="inlineStr"/>
+      <c r="I1108" t="inlineStr"/>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>Title: Fredericksburg Full-Day Guided Trip from Austin</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr"/>
+      <c r="C1109" t="inlineStr"/>
+      <c r="D1109" t="inlineStr"/>
+      <c r="E1109" t="inlineStr"/>
+      <c r="F1109" t="inlineStr"/>
+      <c r="G1109" t="inlineStr"/>
+      <c r="H1109" t="inlineStr"/>
+      <c r="I1109" t="inlineStr"/>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>TotalReviews: 0</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr"/>
+      <c r="C1110" t="inlineStr"/>
+      <c r="D1110" t="inlineStr"/>
+      <c r="E1110" t="inlineStr"/>
+      <c r="F1110" t="inlineStr"/>
+      <c r="G1110" t="inlineStr"/>
+      <c r="H1110" t="inlineStr"/>
+      <c r="I1110" t="inlineStr"/>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>Category: ['Scenic Tours', 'Historical Tours']</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr"/>
+      <c r="C1111" t="inlineStr"/>
+      <c r="D1111" t="inlineStr"/>
+      <c r="E1111" t="inlineStr"/>
+      <c r="F1111" t="inlineStr"/>
+      <c r="G1111" t="inlineStr"/>
+      <c r="H1111" t="inlineStr"/>
+      <c r="I1111" t="inlineStr"/>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>*****</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr"/>
+      <c r="C1112" t="inlineStr"/>
+      <c r="D1112" t="inlineStr"/>
+      <c r="E1112" t="inlineStr"/>
+      <c r="F1112" t="inlineStr"/>
+      <c r="G1112" t="inlineStr"/>
+      <c r="H1112" t="inlineStr"/>
+      <c r="I1112" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>